<commit_message>
relations have been copied to the wrong directories
</commit_message>
<xml_diff>
--- a/test_result_replacement.xlsx
+++ b/test_result_replacement.xlsx
@@ -221,90 +221,6 @@
         <v>2</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="4">
-      <c r="E4" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="5">
-      <c r="B5" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="6">
-      <c r="A6" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="7">
-      <c r="C7" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="8">
-      <c r="C8" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="9">
-      <c r="A9" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink display="http://example.com" ref="E4" r:id="rId1"/>
-  </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Normal"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Normal"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-  <drawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F9"/>
-  <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="60">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.4862745098039"/>
-  </cols>
-  <sheetData>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="1">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="2">
-      <c r="F2" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13" outlineLevel="0" r="3">
-      <c r="B3" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="0" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>